<commit_message>
adding photos and expanding maps
</commit_message>
<xml_diff>
--- a/dev/IssueMap_manual.xlsx
+++ b/dev/IssueMap_manual.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Keith Yoder\repos\SocialValuesTask\dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C4F2D8A0-5C8E-4DC7-BC0F-7AA6BBC3CE89}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7838264C-5CF1-4C99-9382-FD3B7998E1F3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-17865" yWindow="1620" windowWidth="17685" windowHeight="13875" xr2:uid="{C19661DF-E636-41D1-850F-C723F112731C}"/>
+    <workbookView xWindow="-25245" yWindow="720" windowWidth="24360" windowHeight="13995" xr2:uid="{C19661DF-E636-41D1-850F-C723F112731C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="150">
   <si>
     <t>Mask</t>
   </si>
@@ -36,15 +36,6 @@
     <t>Issue</t>
   </si>
   <si>
-    <t>For</t>
-  </si>
-  <si>
-    <t>Against</t>
-  </si>
-  <si>
-    <t>1002_01, 1002_02, 1003_01, 1003_02</t>
-  </si>
-  <si>
     <t>Confederate</t>
   </si>
   <si>
@@ -291,9 +282,6 @@
     <t>DeinvestFossil</t>
   </si>
   <si>
-    <t>Deinvest in Fossil Fuel</t>
-  </si>
-  <si>
     <t>ProtestRights</t>
   </si>
   <si>
@@ -330,10 +318,163 @@
     <t>More government benefits during COVID pandemic</t>
   </si>
   <si>
-    <t>Police Brutality</t>
-  </si>
-  <si>
     <t>Drones</t>
+  </si>
+  <si>
+    <t>For1</t>
+  </si>
+  <si>
+    <t>Against1</t>
+  </si>
+  <si>
+    <t>For2</t>
+  </si>
+  <si>
+    <t>Against2</t>
+  </si>
+  <si>
+    <t>Stop police brutality</t>
+  </si>
+  <si>
+    <t>Divest from Fossil Fuels</t>
+  </si>
+  <si>
+    <t>1026_01</t>
+  </si>
+  <si>
+    <t>1026_02</t>
+  </si>
+  <si>
+    <t>1027_01</t>
+  </si>
+  <si>
+    <t>1027_02</t>
+  </si>
+  <si>
+    <t>1034_01</t>
+  </si>
+  <si>
+    <t>1035_05</t>
+  </si>
+  <si>
+    <t>1017_01</t>
+  </si>
+  <si>
+    <t>1017_02</t>
+  </si>
+  <si>
+    <t>1024_01</t>
+  </si>
+  <si>
+    <t>1035_02</t>
+  </si>
+  <si>
+    <t>1036_01</t>
+  </si>
+  <si>
+    <t>1039_02</t>
+  </si>
+  <si>
+    <t>1045_02</t>
+  </si>
+  <si>
+    <t>1048_01</t>
+  </si>
+  <si>
+    <t>1048_02</t>
+  </si>
+  <si>
+    <t>1076_01</t>
+  </si>
+  <si>
+    <t>1065_01</t>
+  </si>
+  <si>
+    <t>1002_01</t>
+  </si>
+  <si>
+    <t>1002_02</t>
+  </si>
+  <si>
+    <t>1003_02</t>
+  </si>
+  <si>
+    <t>1003_01</t>
+  </si>
+  <si>
+    <t>1018_01</t>
+  </si>
+  <si>
+    <t>1019_01</t>
+  </si>
+  <si>
+    <t>1007_02</t>
+  </si>
+  <si>
+    <t>1021_01</t>
+  </si>
+  <si>
+    <t>1021_02</t>
+  </si>
+  <si>
+    <t>1005_02</t>
+  </si>
+  <si>
+    <t>1007_01</t>
+  </si>
+  <si>
+    <t>1008_01</t>
+  </si>
+  <si>
+    <t>1008_02</t>
+  </si>
+  <si>
+    <t>1020_02</t>
+  </si>
+  <si>
+    <t>1020_01</t>
+  </si>
+  <si>
+    <t>1034_02</t>
+  </si>
+  <si>
+    <t>1047_01</t>
+  </si>
+  <si>
+    <t>1068_01</t>
+  </si>
+  <si>
+    <t>1076_02</t>
+  </si>
+  <si>
+    <t>1047_02</t>
+  </si>
+  <si>
+    <t>1005_01</t>
+  </si>
+  <si>
+    <t>1006_01</t>
+  </si>
+  <si>
+    <t>1006_02</t>
+  </si>
+  <si>
+    <t>1011_01</t>
+  </si>
+  <si>
+    <t>1011_02</t>
+  </si>
+  <si>
+    <t>1035_03</t>
+  </si>
+  <si>
+    <t>1059_01</t>
+  </si>
+  <si>
+    <t>MinimumWage</t>
+  </si>
+  <si>
+    <t>Raise the minimum wage</t>
   </si>
 </sst>
 </file>
@@ -381,15 +522,42 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -699,19 +867,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C75A9C2-F948-4BA5-944A-A99ECB2770D2}">
-  <dimension ref="A1:D50"/>
+  <dimension ref="A1:F51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="54.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -719,408 +890,809 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="F1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
+      <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="C2" s="3">
+        <v>1050</v>
+      </c>
+      <c r="D2">
+        <v>351</v>
+      </c>
+      <c r="E2" s="3">
+        <v>1001</v>
+      </c>
+      <c r="F2">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C3" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="D3" s="1">
+        <v>1042</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="B4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C4" s="3">
+        <v>262</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="F4">
+        <v>1054</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="B5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C5" s="3">
+        <v>275</v>
+      </c>
+      <c r="D5">
+        <v>366</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="B6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="C6" s="3">
+        <v>282</v>
+      </c>
+      <c r="D6" t="s">
+        <v>145</v>
+      </c>
+      <c r="E6" s="3">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="B7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="C7" s="3">
+        <v>1001</v>
+      </c>
+      <c r="E7" s="3">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="B8" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="C8" s="3">
+        <v>362</v>
+      </c>
+      <c r="D8">
+        <v>315</v>
+      </c>
+      <c r="E8" s="3">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="C9" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="E9" s="3">
+        <v>280</v>
+      </c>
+      <c r="F9">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="B10" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="C10" s="3">
+        <v>1016</v>
+      </c>
+      <c r="D10" t="s">
+        <v>144</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="B11" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="C11" s="3">
+        <v>320</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+      <c r="B12" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="C12" s="3">
+        <v>316</v>
+      </c>
+      <c r="E12" s="3">
+        <v>1080</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+      <c r="B13" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="C13" s="3">
+        <v>1014</v>
+      </c>
+      <c r="D13" t="s">
+        <v>142</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+      <c r="B14" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="C14" s="3">
+        <v>272</v>
+      </c>
+      <c r="D14" t="s">
+        <v>141</v>
+      </c>
+      <c r="E14" s="3">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+      <c r="B15" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="C15" s="3">
+        <v>254</v>
+      </c>
+      <c r="E15" s="3">
+        <v>369</v>
+      </c>
+      <c r="F15">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+      <c r="B16" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="C16" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="E16" s="3">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+      <c r="B17" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C17" s="3">
+        <v>367</v>
+      </c>
+      <c r="D17">
+        <v>288</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B18" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
+      <c r="C18" s="3">
+        <v>341</v>
+      </c>
+      <c r="E18" s="3">
+        <v>1075</v>
+      </c>
+      <c r="F18" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
+      <c r="B19" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="C19" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="E19" s="3">
+        <v>300</v>
+      </c>
+      <c r="F19">
+        <v>1077</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+      <c r="B20" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="C20" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="E20" s="3">
+        <v>999</v>
+      </c>
+      <c r="F20" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
+      <c r="B21" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="C21" s="3">
+        <v>202</v>
+      </c>
+      <c r="D21">
+        <v>216</v>
+      </c>
+      <c r="E21" s="3">
+        <v>377</v>
+      </c>
+      <c r="F21" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
+      <c r="B22" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="C22" s="3">
+        <v>374</v>
+      </c>
+      <c r="D22">
+        <v>378</v>
+      </c>
+      <c r="E22" s="3">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
+      <c r="B23" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="C23" s="3">
+        <v>217</v>
+      </c>
+      <c r="D23">
+        <v>289</v>
+      </c>
+      <c r="E23" s="3">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
+      <c r="B24" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="C24" s="3">
+        <v>257</v>
+      </c>
+      <c r="D24">
+        <v>1073</v>
+      </c>
+      <c r="E24" s="3">
+        <v>206</v>
+      </c>
+      <c r="F24">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
+      <c r="B25" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="C25" s="3">
+        <v>230</v>
+      </c>
+      <c r="E25" s="3">
+        <v>1082</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
+      <c r="B26" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="C26" s="3">
+        <v>1038</v>
+      </c>
+      <c r="E26" s="3">
+        <v>1081</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
+      <c r="B27" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="C27" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="E27" s="3">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
+      <c r="B28" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="C28" s="3">
+        <v>1077</v>
+      </c>
+      <c r="E28" s="3">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B29" s="1" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
+      <c r="C29" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="F29">
+        <v>1023</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B30" s="1" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="B29" s="1" t="s">
+      <c r="C30" s="3">
+        <v>297</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
+      <c r="B31" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="C31" s="3">
+        <v>333</v>
+      </c>
+      <c r="E31" s="3">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
+      <c r="B32" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="C32" s="3">
+        <v>268</v>
+      </c>
+      <c r="E32" s="3">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
+      <c r="B33" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="C33" s="3">
+        <v>1079</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
+      <c r="B34" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B33" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C34" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B35" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="D35" t="s">
+        <v>123</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="E36" s="3">
+        <v>1001</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C37" s="3"/>
+      <c r="E37" s="3"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C38" s="3">
+        <v>368</v>
+      </c>
+      <c r="E38" s="3">
+        <v>1004</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C39" s="3">
+        <v>1078</v>
+      </c>
+      <c r="D39" t="s">
+        <v>119</v>
+      </c>
+      <c r="E39" s="3"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C40" s="3"/>
+      <c r="E40" s="3"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="D41" t="s">
+        <v>111</v>
+      </c>
+      <c r="E41" s="3">
+        <v>1083</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C42" s="3">
+        <v>1014</v>
+      </c>
+      <c r="D42">
+        <v>1033</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="F42" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="D43">
+        <v>1041</v>
+      </c>
+      <c r="E43" s="3"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B44" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="C35" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="B38" s="1" t="s">
+      <c r="C44" s="3">
+        <v>1084</v>
+      </c>
+      <c r="D44" t="s">
+        <v>147</v>
+      </c>
+      <c r="E44" s="3">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B45" s="2" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="B41" s="1" t="s">
+      <c r="C45" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="D45">
+        <v>1010</v>
+      </c>
+      <c r="E45" s="3">
+        <v>1032</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C46" s="3"/>
+      <c r="E46" s="3"/>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C47" s="3"/>
+      <c r="E47" s="3" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="D48">
+        <v>1009</v>
+      </c>
+      <c r="E48" s="3"/>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B49" s="2" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="B43" s="2" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="B47" s="2" t="s">
+      <c r="C49" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="D49" t="s">
+        <v>118</v>
+      </c>
+      <c r="E49" s="3"/>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="B49" s="2" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" s="2" t="s">
-        <v>92</v>
-      </c>
       <c r="B50" s="2" t="s">
-        <v>101</v>
+        <v>102</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="E50" s="3">
+        <v>231</v>
+      </c>
+      <c r="F50" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>147</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="C2:C29 E1:E50 C31:C51">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="lessThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C30">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>